<commit_message>
actual response error need to be fixed
</commit_message>
<xml_diff>
--- a/Reports/Chatbot_Test_Results.xlsx
+++ b/Reports/Chatbot_Test_Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
   <si>
     <t>TestID</t>
   </si>
@@ -222,21 +222,55 @@
     <t>Can you please type your question?</t>
   </si>
   <si>
-    <t>Error: Expected condition failed: waiting for element to be clickable: By.xpath: //input[@placeholder='Type a message' or @placeholder='Ask me anything...' or contains(@class, 'input')] (tried for 15 second(s) with 500 milliseconds interval)
-Build info: version: '4.25.0', revision: '8a8aea2337'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.22'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 139.0.7258.128, chrome: {chromedriverVersion: 139.0.7258.138 (884e54ea8d4..., userDataDir: C:\WINDOWS\SystemTemp\scope...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:59258}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:59258/devtoo..., se:cdpVersion: 139.0.7258.128, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: b264c4942ab6f2f85f396115d23164f9</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>Hello / Hi Good day! What can I do for you today?</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>What are your working hours? We are open 9  to 5 , Monday to Friday.</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Where are you located? Sorry, could you say that again?</t>
+  </si>
+  <si>
+    <t>What is your contact number? You can email support@example.com or call 123-456-7890.</t>
+  </si>
+  <si>
+    <t>Thanks / Thank you I didn't get that. Can you repeat?</t>
+  </si>
+  <si>
+    <t>Blah blah blah What was that?</t>
+  </si>
+  <si>
+    <t>Wht are ur hours? We are open 9  to 5 , Monday to Friday.</t>
+  </si>
+  <si>
+    <t>What services do you offer? Can you say that again?</t>
+  </si>
+  <si>
+    <t>What is the price of [Service]? One more time?</t>
+  </si>
+  <si>
+    <t>How can I contact support? For support, email support@example.com or call 123-456-7890.</t>
+  </si>
+  <si>
+    <t>What is your email? Sorry, what was that?</t>
+  </si>
+  <si>
+    <t>Hey there! Hello! How can I help you today?</t>
+  </si>
+  <si>
+    <t>When do you close? Sorry, could you say that again?</t>
+  </si>
+  <si>
+    <t>When do you open? We are open 9  to 5 , Monday to Friday.</t>
+  </si>
+  <si>
+    <t>"" (no input) I didn't get that. Can you say it again?</t>
   </si>
 </sst>
 </file>
@@ -620,9 +654,12 @@
         <v>36</v>
       </c>
       <c r="D2" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -637,10 +674,13 @@
         <v>37</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -654,9 +694,12 @@
         <v>38</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -671,9 +714,12 @@
         <v>39</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -688,9 +734,12 @@
         <v>40</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -705,9 +754,12 @@
         <v>41</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -722,9 +774,12 @@
         <v>42</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -739,10 +794,13 @@
         <v>43</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -756,9 +814,12 @@
         <v>44</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -773,10 +834,13 @@
         <v>45</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -789,11 +853,14 @@
       <c r="C12" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="D12" t="s" s="0">
-        <v>67</v>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>68</v>
+        <v>77</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -807,10 +874,13 @@
         <v>47</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>68</v>
+        <v>78</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -824,10 +894,13 @@
         <v>48</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>68</v>
+        <v>79</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -841,9 +914,12 @@
         <v>49</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -858,10 +934,13 @@
         <v>50</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>68</v>
+        <v>81</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>